<commit_message>
Fix #4006 Model MAGE-TABv1.0.xlsx import error
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/MAGE-TABv1.0.xlsx
+++ b/molgenis-model-registry/src/test/resources/MAGE-TABv1.0.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="31660" windowHeight="19420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="135" yWindow="0" windowWidth="29040" windowHeight="18240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="357">
   <si>
     <t>Investigation Description Format</t>
   </si>
@@ -808,13 +808,298 @@
   </si>
   <si>
     <t>magetab_data</t>
+  </si>
+  <si>
+    <t>MAGE1</t>
+  </si>
+  <si>
+    <t>MAGE2</t>
+  </si>
+  <si>
+    <t>MAGE3</t>
+  </si>
+  <si>
+    <t>MAGE4</t>
+  </si>
+  <si>
+    <t>MAGE5</t>
+  </si>
+  <si>
+    <t>MAGE6</t>
+  </si>
+  <si>
+    <t>MAGE7</t>
+  </si>
+  <si>
+    <t>MAGE8</t>
+  </si>
+  <si>
+    <t>MAGE9</t>
+  </si>
+  <si>
+    <t>MAGE10</t>
+  </si>
+  <si>
+    <t>MAGE11</t>
+  </si>
+  <si>
+    <t>MAGE12</t>
+  </si>
+  <si>
+    <t>MAGE13</t>
+  </si>
+  <si>
+    <t>MAGE14</t>
+  </si>
+  <si>
+    <t>MAGE15</t>
+  </si>
+  <si>
+    <t>MAGE16</t>
+  </si>
+  <si>
+    <t>MAGE17</t>
+  </si>
+  <si>
+    <t>MAGE18</t>
+  </si>
+  <si>
+    <t>MAGE19</t>
+  </si>
+  <si>
+    <t>MAGE20</t>
+  </si>
+  <si>
+    <t>MAGE21</t>
+  </si>
+  <si>
+    <t>MAGE22</t>
+  </si>
+  <si>
+    <t>MAGE23</t>
+  </si>
+  <si>
+    <t>MAGE24</t>
+  </si>
+  <si>
+    <t>MAGE25</t>
+  </si>
+  <si>
+    <t>MAGE26</t>
+  </si>
+  <si>
+    <t>MAGE27</t>
+  </si>
+  <si>
+    <t>MAGE28</t>
+  </si>
+  <si>
+    <t>MAGE29</t>
+  </si>
+  <si>
+    <t>MAGE30</t>
+  </si>
+  <si>
+    <t>MAGE31</t>
+  </si>
+  <si>
+    <t>MAGE32</t>
+  </si>
+  <si>
+    <t>MAGE33</t>
+  </si>
+  <si>
+    <t>MAGE34</t>
+  </si>
+  <si>
+    <t>MAGE35</t>
+  </si>
+  <si>
+    <t>MAGE36</t>
+  </si>
+  <si>
+    <t>MAGE37</t>
+  </si>
+  <si>
+    <t>MAGE38</t>
+  </si>
+  <si>
+    <t>MAGE39</t>
+  </si>
+  <si>
+    <t>MAGE40</t>
+  </si>
+  <si>
+    <t>MAGE41</t>
+  </si>
+  <si>
+    <t>MAGE42</t>
+  </si>
+  <si>
+    <t>MAGE43</t>
+  </si>
+  <si>
+    <t>MAGE44</t>
+  </si>
+  <si>
+    <t>MAGE45</t>
+  </si>
+  <si>
+    <t>MAGE46</t>
+  </si>
+  <si>
+    <t>MAGE47</t>
+  </si>
+  <si>
+    <t>MAGE48</t>
+  </si>
+  <si>
+    <t>MAGE49</t>
+  </si>
+  <si>
+    <t>MAGE50</t>
+  </si>
+  <si>
+    <t>MAGE51</t>
+  </si>
+  <si>
+    <t>MAGE52</t>
+  </si>
+  <si>
+    <t>MAGE53</t>
+  </si>
+  <si>
+    <t>MAGE54</t>
+  </si>
+  <si>
+    <t>MAGE55</t>
+  </si>
+  <si>
+    <t>MAGE56</t>
+  </si>
+  <si>
+    <t>MAGE57</t>
+  </si>
+  <si>
+    <t>MAGE58</t>
+  </si>
+  <si>
+    <t>MAGE59</t>
+  </si>
+  <si>
+    <t>MAGE60</t>
+  </si>
+  <si>
+    <t>MAGE61</t>
+  </si>
+  <si>
+    <t>MAGE62</t>
+  </si>
+  <si>
+    <t>MAGE63</t>
+  </si>
+  <si>
+    <t>MAGE64</t>
+  </si>
+  <si>
+    <t>MAGE65</t>
+  </si>
+  <si>
+    <t>MAGE66</t>
+  </si>
+  <si>
+    <t>MAGE67</t>
+  </si>
+  <si>
+    <t>MAGE68</t>
+  </si>
+  <si>
+    <t>MAGE69</t>
+  </si>
+  <si>
+    <t>MAGE70</t>
+  </si>
+  <si>
+    <t>MAGE71</t>
+  </si>
+  <si>
+    <t>MAGE72</t>
+  </si>
+  <si>
+    <t>MAGE73</t>
+  </si>
+  <si>
+    <t>MAGE74</t>
+  </si>
+  <si>
+    <t>MAGE75</t>
+  </si>
+  <si>
+    <t>MAGE76</t>
+  </si>
+  <si>
+    <t>MAGE77</t>
+  </si>
+  <si>
+    <t>MAGE78</t>
+  </si>
+  <si>
+    <t>MAGE79</t>
+  </si>
+  <si>
+    <t>MAGE80</t>
+  </si>
+  <si>
+    <t>MAGE81</t>
+  </si>
+  <si>
+    <t>MAGE82</t>
+  </si>
+  <si>
+    <t>MAGE83</t>
+  </si>
+  <si>
+    <t>MAGE84</t>
+  </si>
+  <si>
+    <t>MAGE85</t>
+  </si>
+  <si>
+    <t>MAGE86</t>
+  </si>
+  <si>
+    <t>MAGE87</t>
+  </si>
+  <si>
+    <t>MAGE88</t>
+  </si>
+  <si>
+    <t>MAGE89</t>
+  </si>
+  <si>
+    <t>MAGE90</t>
+  </si>
+  <si>
+    <t>MAGE91</t>
+  </si>
+  <si>
+    <t>MAGE92</t>
+  </si>
+  <si>
+    <t>MAGE93</t>
+  </si>
+  <si>
+    <t>MAGE94</t>
+  </si>
+  <si>
+    <t>MAGE95</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1237,6 +1522,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1568,13 +1858,13 @@
       <selection activeCell="A7" sqref="A7:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="85.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.625" customWidth="1"/>
+    <col min="3" max="3" width="85.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1594,7 +1884,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45">
+    <row r="2" spans="1:5" ht="47.25">
       <c r="A2" t="s">
         <v>222</v>
       </c>
@@ -1609,7 +1899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="31.5">
       <c r="A3" t="s">
         <v>223</v>
       </c>
@@ -1624,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="45">
+    <row r="4" spans="1:5" ht="47.25">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -1639,7 +1929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="31.5">
       <c r="A5" t="s">
         <v>225</v>
       </c>
@@ -1682,1522 +1972,1810 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W96"/>
+  <dimension ref="A1:X96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D94" sqref="D94"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="3"/>
-    <col min="6" max="6" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="3"/>
-    <col min="10" max="10" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="3"/>
-    <col min="15" max="15" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="10.83203125" style="3"/>
-    <col min="18" max="18" width="23.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" style="3"/>
-    <col min="20" max="20" width="16.6640625" style="3" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="3"/>
-    <col min="22" max="22" width="26" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="2" width="15" style="3" customWidth="1"/>
+    <col min="3" max="3" width="30" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.875" style="3"/>
+    <col min="7" max="7" width="34.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.875" style="3"/>
+    <col min="11" max="11" width="9.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.875" style="3"/>
+    <col min="16" max="16" width="12.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.875" style="3"/>
+    <col min="19" max="19" width="23.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.875" style="3"/>
+    <col min="21" max="21" width="16.625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="10.875" style="3"/>
+    <col min="23" max="23" width="26" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" s="3" t="s">
         <v>204</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="16">
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="5"/>
+      <c r="S2" s="4"/>
       <c r="T2" s="5"/>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
       <c r="W2" s="5"/>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>258</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18">
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" spans="1:19">
       <c r="A17" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18">
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="1:19">
       <c r="A18" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>258</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18">
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" spans="1:19">
       <c r="A19" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" spans="1:19">
       <c r="A20" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>258</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19">
       <c r="A21" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18">
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19">
       <c r="A22" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>258</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18">
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" spans="1:19">
       <c r="A23" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18">
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" spans="1:19">
       <c r="A24" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="R24" s="2"/>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" spans="1:19">
       <c r="A25" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="R25" s="2"/>
-    </row>
-    <row r="26" spans="1:18">
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="H26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="R26" s="2"/>
-    </row>
-    <row r="27" spans="1:18">
+      <c r="S26" s="2"/>
+    </row>
+    <row r="27" spans="1:19">
       <c r="A27" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="R27" s="2"/>
-    </row>
-    <row r="28" spans="1:18">
+      <c r="S27" s="2"/>
+    </row>
+    <row r="28" spans="1:19">
       <c r="A28" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="R28" s="2"/>
-    </row>
-    <row r="29" spans="1:18">
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" spans="1:19">
       <c r="A29" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="D29"/>
-      <c r="F29" s="3" t="s">
+      <c r="E29"/>
+      <c r="G29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="R29" s="2"/>
-    </row>
-    <row r="30" spans="1:18">
+      <c r="S29" s="2"/>
+    </row>
+    <row r="30" spans="1:19">
       <c r="A30" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>258</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R30" s="2"/>
-    </row>
-    <row r="31" spans="1:18">
+      <c r="S30" s="2"/>
+    </row>
+    <row r="31" spans="1:19">
       <c r="A31" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R31" s="2"/>
-    </row>
-    <row r="32" spans="1:18">
+      <c r="S31" s="2"/>
+    </row>
+    <row r="32" spans="1:19">
       <c r="A32" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E32" s="3" t="b">
+      <c r="F32" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="3" t="b">
+      <c r="I32" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:18">
+      <c r="S32" s="2"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="R33" s="2"/>
-    </row>
-    <row r="34" spans="1:18">
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="R34" s="2"/>
-    </row>
-    <row r="35" spans="1:18">
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="H35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="R35" s="2"/>
-    </row>
-    <row r="36" spans="1:18">
+      <c r="S35" s="2"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="D36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="R36" s="2"/>
-    </row>
-    <row r="37" spans="1:18">
+      <c r="S36" s="2"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18">
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="R38" s="2"/>
-    </row>
-    <row r="39" spans="1:18">
+      <c r="S38" s="2"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>258</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="R39" s="2"/>
-    </row>
-    <row r="40" spans="1:18">
+      <c r="S39" s="2"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="C40" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18">
+      <c r="S40" s="2"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>258</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R41" s="2"/>
-    </row>
-    <row r="42" spans="1:18">
+      <c r="S41" s="2"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>258</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="D42" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="E42" s="3" t="b">
+      <c r="F42" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H42" s="3" t="b">
+      <c r="I42" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="R42" s="2"/>
-    </row>
-    <row r="43" spans="1:18">
+      <c r="S42" s="2"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>258</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="D43" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R43" s="2"/>
-    </row>
-    <row r="44" spans="1:18">
+      <c r="S43" s="2"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="C44" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="D44" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E44" s="3" t="b">
+      <c r="F44" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H44" s="3" t="b">
+      <c r="I44" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18">
+      <c r="S44" s="2"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R45" s="2"/>
-    </row>
-    <row r="46" spans="1:18">
+      <c r="S45" s="2"/>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D46" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18">
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:18">
+      <c r="S47" s="2"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="D48" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18">
+      <c r="S48" s="2"/>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="D49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>258</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="R49" s="2"/>
-    </row>
-    <row r="50" spans="1:18">
+      <c r="S49" s="2"/>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18">
+      <c r="S50" s="2"/>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>258</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="R51" s="2"/>
-    </row>
-    <row r="52" spans="1:18">
+      <c r="S51" s="2"/>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="R52" s="2"/>
-    </row>
-    <row r="53" spans="1:18">
+      <c r="S52" s="2"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="D53" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>258</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="R53" s="2"/>
-    </row>
-    <row r="54" spans="1:18">
+      <c r="S53" s="2"/>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="C54" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="R54" s="2"/>
-    </row>
-    <row r="55" spans="1:18">
+      <c r="S54" s="2"/>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>258</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="R55" s="2"/>
-    </row>
-    <row r="56" spans="1:18">
+      <c r="S55" s="2"/>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R56" s="2"/>
-    </row>
-    <row r="57" spans="1:18">
+      <c r="S56" s="2"/>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="R57" s="2"/>
-    </row>
-    <row r="58" spans="1:18">
+      <c r="S57" s="2"/>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R58" s="2"/>
-    </row>
-    <row r="59" spans="1:18">
+      <c r="S58" s="2"/>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="R59" s="2"/>
-    </row>
-    <row r="60" spans="1:18">
+      <c r="S59" s="2"/>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="R60" s="2"/>
-    </row>
-    <row r="61" spans="1:18">
+      <c r="S60" s="2"/>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="R61" s="2"/>
-    </row>
-    <row r="62" spans="1:18">
+      <c r="S61" s="2"/>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="R62" s="2"/>
-    </row>
-    <row r="63" spans="1:18">
+      <c r="S62" s="2"/>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R63" s="2"/>
-    </row>
-    <row r="64" spans="1:18">
+      <c r="S63" s="2"/>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="D64" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R64" s="2"/>
-    </row>
-    <row r="65" spans="1:18">
+      <c r="S64" s="2"/>
+    </row>
+    <row r="65" spans="1:19">
       <c r="A65" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D65" s="6" t="s">
+      <c r="E65" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R65" s="2"/>
-    </row>
-    <row r="66" spans="1:18">
+      <c r="S65" s="2"/>
+    </row>
+    <row r="66" spans="1:19">
       <c r="A66" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="C66" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R66" s="2"/>
-    </row>
-    <row r="67" spans="1:18">
+      <c r="S66" s="2"/>
+    </row>
+    <row r="67" spans="1:19">
       <c r="A67" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="E67" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R67" s="2"/>
-    </row>
-    <row r="68" spans="1:18">
+      <c r="S67" s="2"/>
+    </row>
+    <row r="68" spans="1:19">
       <c r="A68" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="C68" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R68" s="2"/>
-    </row>
-    <row r="69" spans="1:18">
+      <c r="S68" s="2"/>
+    </row>
+    <row r="69" spans="1:19">
       <c r="A69" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="R69" s="2"/>
-    </row>
-    <row r="70" spans="1:18">
+      <c r="S69" s="2"/>
+    </row>
+    <row r="70" spans="1:19">
       <c r="A70" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="R70" s="2"/>
-    </row>
-    <row r="71" spans="1:18">
+      <c r="S70" s="2"/>
+    </row>
+    <row r="71" spans="1:19">
       <c r="A71" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="G71" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="R71" s="2"/>
-    </row>
-    <row r="72" spans="1:18">
+      <c r="S71" s="2"/>
+    </row>
+    <row r="72" spans="1:19">
       <c r="A72" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="C72" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="D72" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E72" s="3" t="b">
+      <c r="F72" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H72" s="3" t="b">
+      <c r="I72" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="R72" s="2"/>
-    </row>
-    <row r="73" spans="1:18">
+      <c r="S72" s="2"/>
+    </row>
+    <row r="73" spans="1:19">
       <c r="A73" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="C73" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="R73" s="2"/>
-    </row>
-    <row r="74" spans="1:18">
+      <c r="S73" s="2"/>
+    </row>
+    <row r="74" spans="1:19">
       <c r="A74" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="C74" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="R74" s="2"/>
-    </row>
-    <row r="75" spans="1:18">
+      <c r="S74" s="2"/>
+    </row>
+    <row r="75" spans="1:19">
       <c r="A75" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="R75" s="2"/>
-    </row>
-    <row r="76" spans="1:18">
+      <c r="S75" s="2"/>
+    </row>
+    <row r="76" spans="1:19">
       <c r="A76" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R76" s="2"/>
-    </row>
-    <row r="77" spans="1:18">
+      <c r="S76" s="2"/>
+    </row>
+    <row r="77" spans="1:19">
       <c r="A77" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="R77" s="2"/>
-    </row>
-    <row r="78" spans="1:18">
+      <c r="S77" s="2"/>
+    </row>
+    <row r="78" spans="1:19">
       <c r="A78" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="R78" s="2"/>
-    </row>
-    <row r="79" spans="1:18">
+      <c r="S78" s="2"/>
+    </row>
+    <row r="79" spans="1:19">
       <c r="A79" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="C79" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="R79" s="2"/>
-    </row>
-    <row r="80" spans="1:18">
+      <c r="S79" s="2"/>
+    </row>
+    <row r="80" spans="1:19">
       <c r="A80" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="C80" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F80" s="3" t="s">
+      <c r="G80" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="R80" s="2"/>
-    </row>
-    <row r="81" spans="1:18">
+      <c r="S80" s="2"/>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="C81" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F81" s="3" t="s">
+      <c r="G81" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="R81" s="2"/>
-    </row>
-    <row r="82" spans="1:18">
+      <c r="S81" s="2"/>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="C82" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F82" s="3" t="s">
+      <c r="G82" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="R82" s="2"/>
-    </row>
-    <row r="83" spans="1:18">
+      <c r="S82" s="2"/>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="3" t="s">
+      <c r="C83" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="R83" s="2"/>
-    </row>
-    <row r="84" spans="1:18">
+      <c r="S83" s="2"/>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R84" s="2"/>
-    </row>
-    <row r="85" spans="1:18">
+      <c r="S84" s="2"/>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="C85" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="D85" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="R85" s="2"/>
-    </row>
-    <row r="86" spans="1:18">
+      <c r="S85" s="2"/>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="C86" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R86" s="2"/>
-    </row>
-    <row r="87" spans="1:18">
+      <c r="S86" s="2"/>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="R87" s="2"/>
-    </row>
-    <row r="88" spans="1:18">
+      <c r="S87" s="2"/>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F88" s="3" t="s">
+      <c r="G88" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="R88" s="2"/>
-    </row>
-    <row r="89" spans="1:18">
+      <c r="S88" s="2"/>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F89" s="3" t="s">
+      <c r="G89" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="R89" s="2"/>
-    </row>
-    <row r="90" spans="1:18">
+      <c r="S89" s="2"/>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="C90" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F90" s="3" t="s">
+      <c r="G90" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="R90" s="2"/>
-    </row>
-    <row r="91" spans="1:18">
+      <c r="S90" s="2"/>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="D91" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F91" s="3" t="s">
+      <c r="G91" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R91" s="2"/>
-    </row>
-    <row r="92" spans="1:18">
+      <c r="S91" s="2"/>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F92" s="3" t="s">
+      <c r="G92" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R92" s="2"/>
-    </row>
-    <row r="93" spans="1:18">
+      <c r="S92" s="2"/>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R93" s="2"/>
-    </row>
-    <row r="94" spans="1:18">
+      <c r="S93" s="2"/>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="D94" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D94" s="6" t="s">
+      <c r="E94" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="R94" s="2"/>
-    </row>
-    <row r="95" spans="1:18">
+      <c r="S94" s="2"/>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B95" s="3" t="s">
+      <c r="C95" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E95" s="3" t="b">
+      <c r="F95" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="H95" s="3" t="b">
+      <c r="I95" s="3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:18">
+    <row r="96" spans="1:19">
       <c r="A96" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B96" s="3" t="s">
+      <c r="C96" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="C96" s="3" t="s">
+      <c r="D96" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>231</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"xref"</formula>
     </cfRule>
@@ -3220,9 +3798,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="4" max="4" width="36.1640625" customWidth="1"/>
+    <col min="4" max="4" width="36.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3270,10 +3848,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="3" width="64.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="2" max="3" width="64.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>